<commit_message>
Small fixes to prepare delivery
</commit_message>
<xml_diff>
--- a/Subtask5/04-eli-dl-ap-ep-documents/04-SHACL/Documents-Shapes.xlsx
+++ b/Subtask5/04-eli-dl-ap-ep-documents/04-SHACL/Documents-Shapes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="194">
   <si>
     <t xml:space="preserve">Shapes URI</t>
   </si>
@@ -512,49 +512,53 @@
     <t xml:space="preserve">elidl-ep:amends</t>
   </si>
   <si>
-    <t xml:space="preserve">Note : no specifc range constraint is defined as a lot of values are outside the scope of the dataset</t>
+    <t xml:space="preserve">Note : no specifc range constraint is defined as a lot of values are outside the scope of the dataset.
+Min cardinality set to 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eli-dl:amends_draft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min cardinality set to 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eli-dl:DraftLegislationWork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elidl-ep:amendsReportOnAmendments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eli-dl:draft_amended_by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elidl-ep:hasWorkContribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elidl-ep:workHasVoteResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elidl-ep:workCorrects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owl:sameAs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraints on Expressions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eli:realizes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note : changed the range to  LegislativeProcessWork instead of Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elidl-ep:expressionCorrects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eli:language</t>
   </si>
   <si>
     <t xml:space="preserve">1..n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eli-dl:amends_draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eli-dl:DraftLegislationWork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elidl-ep:amendsReportOnAmendments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eli-dl:draft_amended_by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elidl-ep:hasWorkContribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elidl-ep:workHasVoteResult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elidl-ep:workCorrects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">owl:sameAs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraints on Expressions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eli:realizes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note : changed the range to  LegislativeProcessWork instead of Work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elidl-ep:expressionCorrects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eli:language</t>
   </si>
   <si>
     <t xml:space="preserve">eli:title</t>
@@ -970,7 +974,7 @@
       <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.59"/>
@@ -1706,13 +1710,13 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="G109" activeCellId="0" sqref="G109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="8" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.54"/>
@@ -2709,7 +2713,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A39))</f>
         <v>epsh:P39</v>
@@ -2724,11 +2728,11 @@
         <v>163</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="I39" s="1" t="str">
         <f aca="false">LEFT(H39,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" s="0" t="str">
         <f aca="false">IF(OR(RIGHT(H39,1) = "n", RIGHT(H39,1) = "*"),"",RIGHT(H39,1))</f>
@@ -2744,17 +2748,20 @@
         <v>epsh:P40</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C40" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="H40" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I40" s="1" t="str">
         <f aca="false">LEFT(H40,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" s="0" t="str">
         <f aca="false">IF(OR(RIGHT(H40,1) = "n", RIGHT(H40,1) = "*"),"",RIGHT(H40,1))</f>
@@ -3013,7 +3020,7 @@
         <v>51</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="I51" s="1" t="str">
         <f aca="false">LEFT(H51,1)</f>
@@ -3033,13 +3040,13 @@
         <v>epsh:P52</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="I52" s="1" t="str">
         <f aca="false">LEFT(H52,1)</f>
@@ -3050,7 +3057,7 @@
         <v/>
       </c>
       <c r="K52" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3059,7 +3066,7 @@
         <v>epsh:P53</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>51</v>
@@ -3076,7 +3083,7 @@
         <v/>
       </c>
       <c r="K53" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3085,7 +3092,7 @@
         <v>epsh:P54</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>51</v>
@@ -3107,7 +3114,7 @@
     </row>
     <row r="56" s="21" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="21" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U56" s="22"/>
     </row>
@@ -3117,7 +3124,7 @@
         <v>epsh:P57</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>54</v>
@@ -3143,7 +3150,7 @@
         <v>epsh:P58</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>54</v>
@@ -3169,7 +3176,7 @@
         <v>epsh:P59</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>54</v>
@@ -3195,7 +3202,7 @@
         <v>epsh:P60</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>54</v>
@@ -3221,13 +3228,13 @@
         <v>epsh:P61</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>47</v>
@@ -3247,7 +3254,7 @@
     </row>
     <row r="64" s="21" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="21" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="U64" s="22"/>
     </row>
@@ -3257,7 +3264,7 @@
         <v>epsh:P65</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>57</v>
@@ -3283,7 +3290,7 @@
         <v>epsh:P66</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>57</v>
@@ -3309,7 +3316,7 @@
         <v>epsh:P67</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>57</v>

</xml_diff>